<commit_message>
Daysplit is more accurate.
</commit_message>
<xml_diff>
--- a/data_source2.xlsx
+++ b/data_source2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kheyden\Documents\GitHub\Efficiency-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FCEA9A-A03D-4312-A042-4726464168AB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D158B-E344-4160-8E29-0304EEA9B754}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14619" uniqueCount="3426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14641" uniqueCount="3428">
   <si>
     <t>Jairo  Rios</t>
   </si>
@@ -10298,6 +10298,12 @@
   </si>
   <si>
     <t>04/09/18 Mon 12:48 AM</t>
+  </si>
+  <si>
+    <t>04/09/18 Mon 12:54 AM</t>
+  </si>
+  <si>
+    <t>04/09/18 Mon 6:00 AM</t>
   </si>
 </sst>
 </file>
@@ -10637,10 +10643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K1329"/>
+  <dimension ref="A1:K1331"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A1286" workbookViewId="0">
+      <selection activeCell="P1326" sqref="P1326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57163,6 +57169,76 @@
         <v>3048</v>
       </c>
     </row>
+    <row r="1330" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1330" t="s">
+        <v>3426</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1330" t="s">
+        <v>2904</v>
+      </c>
+      <c r="D1330" t="s">
+        <v>2804</v>
+      </c>
+      <c r="E1330" t="s">
+        <v>3046</v>
+      </c>
+      <c r="F1330" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1330" t="s">
+        <v>2942</v>
+      </c>
+      <c r="H1330" t="s">
+        <v>3047</v>
+      </c>
+      <c r="I1330" t="s">
+        <v>2022</v>
+      </c>
+      <c r="J1330" t="s">
+        <v>2950</v>
+      </c>
+      <c r="K1330" t="s">
+        <v>3048</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1331" t="s">
+        <v>3427</v>
+      </c>
+      <c r="B1331" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1331" t="s">
+        <v>2904</v>
+      </c>
+      <c r="D1331" t="s">
+        <v>2804</v>
+      </c>
+      <c r="E1331" t="s">
+        <v>3046</v>
+      </c>
+      <c r="F1331" t="s">
+        <v>2971</v>
+      </c>
+      <c r="G1331" t="s">
+        <v>2942</v>
+      </c>
+      <c r="H1331" t="s">
+        <v>3047</v>
+      </c>
+      <c r="I1331" t="s">
+        <v>2022</v>
+      </c>
+      <c r="J1331" t="s">
+        <v>2950</v>
+      </c>
+      <c r="K1331" t="s">
+        <v>3048</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>